<commit_message>
updated our excela nd added uniqueness metric
this uniqueness metric was added along side its excel counterpart, this is a description on how to name our chart, decsribe what it does and how to deal with it in a tool tip
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/chart_desc_artifact/brief description on charts and tooltips.xlsx
+++ b/Project supporting Artifacts/chart_desc_artifact/brief description on charts and tooltips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/chart_desc_artifact/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22ABF95-91AE-8647-8EF9-EE5D5C2144BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B460B4-246B-B544-B7BA-24DAC8884561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>D3 Chart Name</t>
   </si>
@@ -188,6 +188,18 @@
   </si>
   <si>
     <t>Use to target fields for the 'Fill Missing Values' function to ensure no critical data is missing.</t>
+  </si>
+  <si>
+    <t>uniqueness-metric</t>
+  </si>
+  <si>
+    <t>Uniqueness Metric Chart</t>
+  </si>
+  <si>
+    <t>Displays the level of unique data entries, highlighting potential redundancy in the dataset.</t>
+  </si>
+  <si>
+    <t>Apply 'Collapse Rare Categories' to reduce overfitting in machine learning models and simplify analysis.</t>
   </si>
 </sst>
 </file>
@@ -533,7 +545,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -741,8 +753,18 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="A15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C16" s="5"/>

</xml_diff>

<commit_message>
updated readability metric chart
hey, yet again completed the readability chart , along side this chart i have added a excel counterpart that explain what it does, and how to fix it , improve it using our data cleaning page.
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/chart_desc_artifact/brief description on charts and tooltips.xlsx
+++ b/Project supporting Artifacts/chart_desc_artifact/brief description on charts and tooltips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/chart_desc_artifact/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B460B4-246B-B544-B7BA-24DAC8884561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE89BC95-E8C9-AD4D-A7FE-D5C462FE44DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>D3 Chart Name</t>
   </si>
@@ -200,6 +200,18 @@
   </si>
   <si>
     <t>Apply 'Collapse Rare Categories' to reduce overfitting in machine learning models and simplify analysis.</t>
+  </si>
+  <si>
+    <t>readability-metric</t>
+  </si>
+  <si>
+    <t>Readability Metric Chart</t>
+  </si>
+  <si>
+    <t>Assesses the ease with which data can be read and interpreted by users or processing systems.</t>
+  </si>
+  <si>
+    <t>Utilize 'Trim Whitespace', 'Replace Substrings', and 'Adjust Text Case' to enhance data readability.</t>
   </si>
 </sst>
 </file>
@@ -545,7 +557,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -767,8 +779,18 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="A16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="17" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C17" s="5"/>

</xml_diff>

<commit_message>
updated excel file as requested by sean
used tobi and sean feedback for updating our description and chart tooltip
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/chart_desc_artifact/brief description on charts and tooltips.xlsx
+++ b/Project supporting Artifacts/chart_desc_artifact/brief description on charts and tooltips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/chart_desc_artifact/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190D3BB7-2628-0049-82E5-662A92A8824E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957CB681-4D43-064B-90EE-C0239154EB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>D3 Chart Name</t>
   </si>
@@ -31,18 +31,9 @@
     <t>Chart Description</t>
   </si>
   <si>
-    <t>Tooltip for Data Cleaning</t>
-  </si>
-  <si>
     <t>bubble-chart</t>
   </si>
   <si>
-    <t>Bubble Chart</t>
-  </si>
-  <si>
-    <t>A visual display of data points as bubbles, often used to represent three dimensions of data.</t>
-  </si>
-  <si>
     <t>cardinality</t>
   </si>
   <si>
@@ -76,9 +67,6 @@
     <t>Evaluates data quality across four dimensions: completeness, uniqueness, readability, and consistency, providing a comprehensive overview of data health.</t>
   </si>
   <si>
-    <t>Use this chart to guide specific cleaning actions: Fill missing values for completeness, collapse rare categories for uniqueness, apply regex for readability, and adjust text case or replace substrings for consistency.</t>
-  </si>
-  <si>
     <t>data-types-chart</t>
   </si>
   <si>
@@ -88,21 +76,12 @@
     <t>Categorizes data into different types (numeric, categorical, etc.).</t>
   </si>
   <si>
-    <t>Can inform when to change column types or adjust text case for consistency in categorical data.</t>
-  </si>
-  <si>
     <t>duplicate-chart</t>
   </si>
   <si>
-    <t>Duplicate Chart</t>
-  </si>
-  <si>
     <t>Visualizes the frequency of duplicate records in a dataset.</t>
   </si>
   <si>
-    <t>Spotlights duplicate records to be removed or merged.</t>
-  </si>
-  <si>
     <t>histogram</t>
   </si>
   <si>
@@ -112,33 +91,15 @@
     <t>Represents the distribution of numerical data.</t>
   </si>
   <si>
-    <t>Analyze the distribution of values to inform outlier removal or normalization.</t>
-  </si>
-  <si>
     <t>missing-values-chart</t>
   </si>
   <si>
     <t>Missing Values Chart</t>
   </si>
   <si>
-    <t>Highlights missing data within a dataset.</t>
-  </si>
-  <si>
     <t>Directs where to fill missing values or to decide if a column with too many missing values should be removed.</t>
   </si>
   <si>
-    <t>number-fields-chart</t>
-  </si>
-  <si>
-    <t>Number Fields Chart</t>
-  </si>
-  <si>
-    <t>Displays the count of numeric fields in the dataset.</t>
-  </si>
-  <si>
-    <t>Guides the need for numeric to category conversions or normalization.</t>
-  </si>
-  <si>
     <t>outliers-scatter-plot</t>
   </si>
   <si>
@@ -154,24 +115,12 @@
     <t>records-chart</t>
   </si>
   <si>
-    <t>Records Chart</t>
-  </si>
-  <si>
-    <t>Shows the count of records or entries in the dataset.</t>
-  </si>
-  <si>
-    <t>Assists in identifying if data cleaning has significantly reduced the dataset size, indicating potential over-cleaning.</t>
-  </si>
-  <si>
     <t>spider-chart</t>
   </si>
   <si>
     <t>Spider Chart</t>
   </si>
   <si>
-    <t>A radial chart that shows data in terms of multiple variables.</t>
-  </si>
-  <si>
     <t>Evaluate multiple metrics for a single record to determine data quality and consistency.</t>
   </si>
   <si>
@@ -184,9 +133,6 @@
     <t>Measures the proportion of non-missing entries in the dataset to assess data completeness.</t>
   </si>
   <si>
-    <t>Use to target fields for the 'Fill Missing Values' function to ensure no critical data is missing.</t>
-  </si>
-  <si>
     <t>uniqueness-metric</t>
   </si>
   <si>
@@ -223,14 +169,56 @@
     <t>Correct inconsistencies by 'Changing Column Type', 'Renaming Columns', and using 'Regex' to standardize formats.</t>
   </si>
   <si>
-    <t>Use to identify categorical distribution. Large bubbles may indicate insimetric data points needing normalisation.</t>
+    <t>helptext for Data Cleaning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bubble Chart - Categorical distribution chart </t>
+  </si>
+  <si>
+    <t>Visualises the categorical features within a column as bubbles, used to identify asymmetry.</t>
+  </si>
+  <si>
+    <t>Use to identify categorical distribution. Large bubbles may indicate asimetric data points needing normalisation.</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>shows duplicate records to be removed or merged.</t>
+  </si>
+  <si>
+    <t>Analyze the distribution of values to inform normalization.</t>
+  </si>
+  <si>
+    <t>Highlights the number of missing values within a column in a dataset.</t>
+  </si>
+  <si>
+    <t>number-fields</t>
+  </si>
+  <si>
+    <t>Number Field</t>
+  </si>
+  <si>
+    <t>Displays the count of fields in the dataset.</t>
+  </si>
+  <si>
+    <t>Records</t>
+  </si>
+  <si>
+    <t>Shows the count of entries in the dataset.</t>
+  </si>
+  <si>
+    <t>A radial chart that shows data in terms of multiple variables. decribe what it does more.</t>
+  </si>
+  <si>
+    <t>to improve the score, look into the 'Fill Missing Values' function.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -252,20 +240,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9CB9C"/>
+        <bgColor rgb="FFF9CB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -295,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -312,8 +299,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -364,12 +354,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{96894406-C9B8-DD4A-9975-7C404FDC8156}" name="Table_13" displayName="Table_13" ref="A1:D17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0A899FFA-F12A-124E-8272-A51D85E4C869}" name="Table_1" displayName="Table_1" ref="A1:D17">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{62AA496C-24F8-1E43-B7B0-1A05B811E9A0}" name="D3 Chart Name"/>
-    <tableColumn id="2" xr3:uid="{F08C4309-69DE-A441-900F-066B6899C6C1}" name="Title of Chart"/>
-    <tableColumn id="3" xr3:uid="{01E4C749-92C1-3B41-89E2-C9C772C373BC}" name="Chart Description"/>
-    <tableColumn id="4" xr3:uid="{3DF0D135-640C-6A4C-B8EE-F73E7BE5348B}" name="Tooltip for Data Cleaning"/>
+    <tableColumn id="1" xr3:uid="{A7C9214C-9895-7D4B-9A10-519A0BC3BC13}" name="D3 Chart Name"/>
+    <tableColumn id="2" xr3:uid="{2BD95F68-5228-4F44-B07A-54B74D0761A5}" name="Title of Chart"/>
+    <tableColumn id="3" xr3:uid="{153618ED-1513-8347-BCAD-192818F0FF1B}" name="Chart Description"/>
+    <tableColumn id="4" xr3:uid="{73DD4AD6-215F-AB46-A582-19A1732BE0E7}" name="helptext for Data Cleaning"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -579,7 +569,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -601,231 +591,223 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>67</v>
+        <v>51</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>18</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>38</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>46</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>50</v>
+      <c r="A13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>